<commit_message>
Update algo excel log for LC121 best time to buy and sell stock
</commit_message>
<xml_diff>
--- a/leetcode_progress.xlsx
+++ b/leetcode_progress.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lin/Desktop/Leetcode/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00D2DD7-1088-DB4D-9713-E25B813455FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9117E4E4-BE0A-B849-92FE-93C8B7FF8343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="460" windowWidth="31460" windowHeight="21680" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="460" windowWidth="31460" windowHeight="21680" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="3" r:id="rId1"/>
     <sheet name="64" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="121" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="159">
   <si>
     <t>Problem #</t>
   </si>
@@ -2957,6 +2958,979 @@
       </rPr>
       <t>] ]</t>
     </r>
+  </si>
+  <si>
+    <t>LC121</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Say you have an array for which the ith element is the price of a given stock on day i. If you were only permitted to complete at most one transaction (i.e., buy one and sell one share of the stock), design an algorithm to find the maximum profit.
+Note that you cannot sell a stock before you buy one.</t>
+  </si>
+  <si>
+    <t>[7,1,5,3,6,4]</t>
+  </si>
+  <si>
+    <t>(2HR, 1HR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5      Buy on day 2 (price = 1) and sell on day 5 (price = 6), profit = 6-1 = 5. </t>
+  </si>
+  <si>
+    <t>One Pass Solution O(n) time</t>
+  </si>
+  <si>
+    <t>We track only 2 variables (lowest price, and max profit). We loop through prices array and either update the lowest price (minPrice) or update the max profit (profit)</t>
+  </si>
+  <si>
+    <t>O(n), where n = input prices array length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O(1) </t>
+  </si>
+  <si>
+    <r>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>maxProfit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>prices</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <t>// also initialize profit to lowest possible num so we can reassign later</t>
+  </si>
+  <si>
+    <t>// 2) loop through all prices</t>
+  </si>
+  <si>
+    <t>// update minPrice</t>
+  </si>
+  <si>
+    <r>
+      <t>let</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>minPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Infinity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>let</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>profit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>let</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>prices</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>++) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>let</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>prices</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>];</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>minPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>minPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC586C0"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC586C0"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>minPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>profit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>profit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>minPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>profit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>// 3) track lowest price. if (current price &lt; minPrice)  (always true for 1st loop)</t>
+  </si>
+  <si>
+    <t>// 4) track maxprofit. if (current price - minPrice &gt; profit)</t>
+  </si>
+  <si>
+    <t>// update profit. (price - minPrice) represents the current profit</t>
+  </si>
+  <si>
+    <t>//=&gt; 5</t>
+  </si>
+  <si>
+    <t>//=&gt; 0</t>
+  </si>
+  <si>
+    <r>
+      <t>console</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>maxProfit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">])); </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>console</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>maxProfit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]));</t>
+    </r>
+  </si>
+  <si>
+    <t>// 1) initialize minPrice to largest possible num so we can reassign later</t>
   </si>
 </sst>
 </file>
@@ -3104,7 +4078,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -3233,11 +4207,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3368,6 +4382,12 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3778,7 +4798,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4046,9 +5066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4382,6 +5400,288 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1D8DE8-9A43-6B47-AA06-2D5DAB50FF01}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87" style="2" customWidth="1"/>
+    <col min="3" max="3" width="91.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="20" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="38"/>
+    </row>
+    <row r="10" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="29"/>
+      <c r="B15" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="29"/>
+      <c r="B16" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="33"/>
+    </row>
+    <row r="18" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="29"/>
+      <c r="B18" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="29"/>
+      <c r="B19" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="33"/>
+    </row>
+    <row r="20" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="29"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="32"/>
+    </row>
+    <row r="21" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="29"/>
+      <c r="B21" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="29"/>
+      <c r="B22" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="C23" s="28"/>
+    </row>
+    <row r="24" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="29"/>
+      <c r="B24" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="29"/>
+      <c r="B25" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="29"/>
+      <c r="B26" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="32"/>
+    </row>
+    <row r="27" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="29"/>
+      <c r="B27" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="33"/>
+    </row>
+    <row r="28" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="29"/>
+      <c r="C28" s="32"/>
+    </row>
+    <row r="29" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="29"/>
+      <c r="B29" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="32"/>
+    </row>
+    <row r="30" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="29"/>
+      <c r="B30" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="33"/>
+    </row>
+    <row r="31" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="29"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="33"/>
+    </row>
+    <row r="32" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="29"/>
+      <c r="C32" s="33"/>
+    </row>
+    <row r="33" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="29"/>
+      <c r="B33" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="53"/>
+      <c r="B34" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="29"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>

</xml_diff>